<commit_message>
Modificato il test dei prerequisi
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/prerequisites.xlsx
+++ b/prerequisites/trial prereq/prerequisites.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jcuoncloud-my.sharepoint.com/personal/elettra_scianetti_johncabot_edu/Documents/Documents/advising/prerequisites/trial prereq/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_47E5A3F5F613C8F6C120F4A96FE46A277B9EBB56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2790E2C2-66D4-4691-9CEE-EFB51D8B4620}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Surname</t>
-  </si>
-  <si>
     <t>Course</t>
   </si>
   <si>
-    <t>Requirement Type</t>
+    <t>Type</t>
   </si>
   <si>
     <t>Missing Prerequisite 1</t>
@@ -67,26 +70,38 @@
     <t>Missing Prerequisite 12</t>
   </si>
   <si>
-    <t>Elettra</t>
-  </si>
-  <si>
-    <t>Scianetti</t>
-  </si>
-  <si>
-    <t>Advanced Composition</t>
+    <t>Elettra Scianetti</t>
+  </si>
+  <si>
+    <t>EN 110</t>
   </si>
   <si>
     <t>prerequisite</t>
   </si>
   <si>
-    <t>Mathematical Statistics</t>
+    <t>EN 103.0</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>EN 105.0</t>
+  </si>
+  <si>
+    <t>FIN 372</t>
+  </si>
+  <si>
+    <t>FIN 301.0</t>
+  </si>
+  <si>
+    <t>Grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +163,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +215,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,6 +249,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -260,9 +284,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,14 +460,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,101 +487,154 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>5</v>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check prerequisites and excel print
</commit_message>
<xml_diff>
--- a/prerequisites/trial prereq/prerequisites.xlsx
+++ b/prerequisites/trial prereq/prerequisites.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jcuoncloud-my.sharepoint.com/personal/elettra_scianetti_johncabot_edu/Documents/Documents/advising/prerequisites/trial prereq/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_47E5A3F5F613C8F6C120F4A96FE46A277B9EBB56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2790E2C2-66D4-4691-9CEE-EFB51D8B4620}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -88,20 +82,35 @@
     <t>EN 105.0</t>
   </si>
   <si>
+    <t>EC 480</t>
+  </si>
+  <si>
+    <t>EC 301.0</t>
+  </si>
+  <si>
+    <t>EC 302.0</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>FIN 301.0</t>
+  </si>
+  <si>
+    <t>MA 209.0</t>
+  </si>
+  <si>
+    <t>EC 360.0</t>
+  </si>
+  <si>
     <t>FIN 372</t>
-  </si>
-  <si>
-    <t>FIN 301.0</t>
-  </si>
-  <si>
-    <t>Grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,21 +172,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +216,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -249,7 +250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -284,10 +284,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,17 +459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -603,7 +599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -620,7 +616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -634,7 +630,68 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>